<commit_message>
adicionando model e controller de usuarios
</commit_message>
<xml_diff>
--- a/planilhas/MatrizSod.xlsx
+++ b/planilhas/MatrizSod.xlsx
@@ -424,13 +424,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.85546875" bestFit="1" customWidth="1" min="2" max="2"/>
     <col width="13.140625" bestFit="1" customWidth="1" min="3" max="3"/>
@@ -617,41 +617,6 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>8</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">2 </t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Contabil </t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> SIA</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">4 </t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Admin </t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> SIA</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>

</xml_diff>

<commit_message>
adicioinando cadastro de perfil com verificacao
</commit_message>
<xml_diff>
--- a/planilhas/MatrizSod.xlsx
+++ b/planilhas/MatrizSod.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -424,10 +424,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -483,137 +483,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t xml:space="preserve">2 </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Contabil</t>
+          <t xml:space="preserve"> Contabil </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SAVA</t>
+          <t xml:space="preserve"> SIA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t xml:space="preserve">3 </t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Financeiro</t>
+          <t xml:space="preserve"> Contabil </t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SIA</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">5 </t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Financeiro </t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> SIA</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">3 </t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Contabil </t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
           <t xml:space="preserve"> SAVA</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">5 </t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Financeiro </t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> SIA</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">2 </t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Contabil </t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> SIA</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">3 </t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Contabil </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> SAVA</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">2 </t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Contabil </t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> SIA</t>
         </is>
       </c>
     </row>

</xml_diff>